<commit_message>
Fixed holds in wrong order in grids.csv, etc.
Also made it so that the seq_ratios reordered to match the order of distances between holds, so that everyone's seq_ratios are larger when there's more distance to the next hold
</commit_message>
<xml_diff>
--- a/grid.xlsx
+++ b/grid.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masonyoungblood/Documents/Work/Summer_2021/Speed Climbing/SpeedClimbingABM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E9CD5F-420B-8047-A3E2-6DDAED4C8C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3093E03F-2C24-914A-BAE2-50FC25A5F49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FDE287D6-618D-F84D-BF6F-8BEE7F171CE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="master" sheetId="1" r:id="rId1"/>
+    <sheet name="master" sheetId="5" r:id="rId1"/>
     <sheet name="details" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -493,11 +493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949799B9-FA76-2441-810C-F4DD11A23E85}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEF6326-3916-1C43-BE82-E47C6C6501F8}">
   <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G22"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <f>K2*125</f>
+        <f t="shared" ref="L2:L23" si="0">K2*125</f>
         <v>0</v>
       </c>
       <c r="N2">
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <f>K3*125</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="N3">
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P66" si="0">(9*125*(N3-1))+((N3-1)*(2*187.5))+((O3-1)*125)</f>
+        <f t="shared" ref="P3:P66" si="1">(9*125*(N3-1))+((N3-1)*(2*187.5))+((O3-1)*125)</f>
         <v>1625</v>
       </c>
     </row>
@@ -676,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <f>K4*125</f>
+        <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="N4">
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1750</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="L5">
-        <f>K5*125</f>
+        <f t="shared" si="0"/>
         <v>375</v>
       </c>
       <c r="N5">
@@ -734,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1875</v>
       </c>
     </row>
@@ -772,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <f>K6*125</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="N6">
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
     </row>
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="L7">
-        <f>K7*125</f>
+        <f t="shared" si="0"/>
         <v>625</v>
       </c>
       <c r="N7">
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2125</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="L8">
-        <f>K8*125</f>
+        <f t="shared" si="0"/>
         <v>750</v>
       </c>
       <c r="N8">
@@ -878,7 +878,7 @@
         <v>7</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2250</v>
       </c>
     </row>
@@ -916,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="L9">
-        <f>K9*125</f>
+        <f t="shared" si="0"/>
         <v>875</v>
       </c>
       <c r="N9">
@@ -926,7 +926,7 @@
         <v>8</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2375</v>
       </c>
     </row>
@@ -964,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="L10">
-        <f>K10*125</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="N10">
@@ -974,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
         <v>9</v>
       </c>
       <c r="L11">
-        <f>K11*125</f>
+        <f t="shared" si="0"/>
         <v>1125</v>
       </c>
       <c r="N11">
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2625</v>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
         <v>10</v>
       </c>
       <c r="L12">
-        <f>K12*125</f>
+        <f t="shared" si="0"/>
         <v>1250</v>
       </c>
       <c r="N12">
@@ -1070,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
         <v>12</v>
       </c>
       <c r="L13">
-        <f>K13*125</f>
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
       <c r="N13">
@@ -1118,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="P13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3125</v>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
         <v>13</v>
       </c>
       <c r="L14">
-        <f>K14*125</f>
+        <f t="shared" si="0"/>
         <v>1625</v>
       </c>
       <c r="N14">
@@ -1166,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3250</v>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
         <v>14</v>
       </c>
       <c r="L15">
-        <f>K15*125</f>
+        <f t="shared" si="0"/>
         <v>1750</v>
       </c>
       <c r="N15">
@@ -1214,7 +1214,7 @@
         <v>4</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3375</v>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
         <v>15</v>
       </c>
       <c r="L16">
-        <f>K16*125</f>
+        <f t="shared" si="0"/>
         <v>1875</v>
       </c>
       <c r="N16">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3500</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
         <v>16</v>
       </c>
       <c r="L17">
-        <f>K17*125</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="N17">
@@ -1310,7 +1310,7 @@
         <v>6</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3625</v>
       </c>
     </row>
@@ -1348,7 +1348,7 @@
         <v>17</v>
       </c>
       <c r="L18">
-        <f>K18*125</f>
+        <f t="shared" si="0"/>
         <v>2125</v>
       </c>
       <c r="N18">
@@ -1358,7 +1358,7 @@
         <v>7</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3750</v>
       </c>
     </row>
@@ -1367,24 +1367,24 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F19" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">INDIRECT(ADDRESS(MATCH(1,(B19=$I$1:$I$23)*(D19=$J$1:$J$23),0), 12))</f>
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="G19" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(MATCH(1, (C19=$N$1:$N$91)*(E19=$O$1:$O$91), 0), 16))</f>
-        <v>13125</v>
+        <v>12125</v>
       </c>
       <c r="I19" t="s">
         <v>7</v>
@@ -1396,7 +1396,7 @@
         <v>18</v>
       </c>
       <c r="L19">
-        <f>K19*125</f>
+        <f t="shared" si="0"/>
         <v>2250</v>
       </c>
       <c r="N19">
@@ -1406,7 +1406,7 @@
         <v>8</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3875</v>
       </c>
     </row>
@@ -1421,18 +1421,18 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F20" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">INDIRECT(ADDRESS(MATCH(1,(B20=$I$1:$I$23)*(D20=$J$1:$J$23),0), 12))</f>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="G20" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(MATCH(1, (C20=$N$1:$N$91)*(E20=$O$1:$O$91), 0), 16))</f>
-        <v>12125</v>
+        <v>12750</v>
       </c>
       <c r="I20" t="s">
         <v>7</v>
@@ -1444,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="L20">
-        <f>K20*125</f>
+        <f t="shared" si="0"/>
         <v>2375</v>
       </c>
       <c r="N20">
@@ -1454,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
     </row>
@@ -1463,24 +1463,24 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E21">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F21" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">INDIRECT(ADDRESS(MATCH(1,(B21=$I$1:$I$23)*(D21=$J$1:$J$23),0), 12))</f>
-        <v>2000</v>
+        <v>1250</v>
       </c>
       <c r="G21" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(MATCH(1, (C21=$N$1:$N$91)*(E21=$O$1:$O$91), 0), 16))</f>
-        <v>12750</v>
+        <v>13125</v>
       </c>
       <c r="I21" t="s">
         <v>7</v>
@@ -1492,7 +1492,7 @@
         <v>20</v>
       </c>
       <c r="L21">
-        <f>K21*125</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="N21">
@@ -1502,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="P21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4125</v>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
         <v>21</v>
       </c>
       <c r="L22">
-        <f>K22*125</f>
+        <f t="shared" si="0"/>
         <v>2625</v>
       </c>
       <c r="N22">
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="P22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4500</v>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
         <v>22</v>
       </c>
       <c r="L23">
-        <f>K23*125</f>
+        <f t="shared" si="0"/>
         <v>2750</v>
       </c>
       <c r="N23">
@@ -1575,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4625</v>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="P24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4750</v>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
         <v>4</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4875</v>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
         <v>5</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5125</v>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5250</v>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
         <v>8</v>
       </c>
       <c r="P29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5375</v>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
         <v>9</v>
       </c>
       <c r="P30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5500</v>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
         <v>10</v>
       </c>
       <c r="P31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5625</v>
       </c>
     </row>
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="P32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6000</v>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="P33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6125</v>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="P34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6250</v>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
         <v>4</v>
       </c>
       <c r="P35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6375</v>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="P36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6500</v>
       </c>
     </row>
@@ -1743,7 +1743,7 @@
         <v>6</v>
       </c>
       <c r="P37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6625</v>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
         <v>7</v>
       </c>
       <c r="P38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="P39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6875</v>
       </c>
     </row>
@@ -1779,7 +1779,7 @@
         <v>9</v>
       </c>
       <c r="P40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7000</v>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="P41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7125</v>
       </c>
     </row>
@@ -1803,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="P42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7500</v>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="P43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7625</v>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="P44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7750</v>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
         <v>4</v>
       </c>
       <c r="P45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7875</v>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
       <c r="P46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8000</v>
       </c>
     </row>
@@ -1863,7 +1863,7 @@
         <v>6</v>
       </c>
       <c r="P47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8125</v>
       </c>
     </row>
@@ -1875,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="P48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8250</v>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
         <v>8</v>
       </c>
       <c r="P49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8375</v>
       </c>
     </row>
@@ -1899,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="P50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8500</v>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
         <v>10</v>
       </c>
       <c r="P51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8625</v>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="P52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9000</v>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
         <v>2</v>
       </c>
       <c r="P53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9125</v>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="P54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9250</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
         <v>4</v>
       </c>
       <c r="P55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9375</v>
       </c>
     </row>
@@ -1971,7 +1971,7 @@
         <v>5</v>
       </c>
       <c r="P56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9500</v>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
         <v>6</v>
       </c>
       <c r="P57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9625</v>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="P58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9750</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
         <v>8</v>
       </c>
       <c r="P59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9875</v>
       </c>
     </row>
@@ -2019,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="P60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
         <v>10</v>
       </c>
       <c r="P61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10125</v>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="P62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10500</v>
       </c>
     </row>
@@ -2055,7 +2055,7 @@
         <v>2</v>
       </c>
       <c r="P63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10625</v>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="P64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10750</v>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
         <v>4</v>
       </c>
       <c r="P65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10875</v>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
         <v>5</v>
       </c>
       <c r="P66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11000</v>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
         <v>6</v>
       </c>
       <c r="P67">
-        <f t="shared" ref="P67:P91" si="1">(9*125*(N67-1))+((N67-1)*(2*187.5))+((O67-1)*125)</f>
+        <f t="shared" ref="P67:P91" si="2">(9*125*(N67-1))+((N67-1)*(2*187.5))+((O67-1)*125)</f>
         <v>11125</v>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
         <v>7</v>
       </c>
       <c r="P68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11250</v>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="P69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11375</v>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="P70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11500</v>
       </c>
     </row>
@@ -2151,7 +2151,7 @@
         <v>10</v>
       </c>
       <c r="P71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11625</v>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="P72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12000</v>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
         <v>2</v>
       </c>
       <c r="P73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12125</v>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
         <v>3</v>
       </c>
       <c r="P74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12250</v>
       </c>
     </row>
@@ -2199,7 +2199,7 @@
         <v>4</v>
       </c>
       <c r="P75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12375</v>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="P76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
     </row>
@@ -2223,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="P77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12625</v>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="P78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12750</v>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
         <v>8</v>
       </c>
       <c r="P79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12875</v>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
         <v>9</v>
       </c>
       <c r="P80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13000</v>
       </c>
     </row>
@@ -2271,7 +2271,7 @@
         <v>10</v>
       </c>
       <c r="P81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13125</v>
       </c>
     </row>
@@ -2283,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="P82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13500</v>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
         <v>2</v>
       </c>
       <c r="P83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13625</v>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="P84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13750</v>
       </c>
     </row>
@@ -2319,7 +2319,7 @@
         <v>4</v>
       </c>
       <c r="P85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13875</v>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
         <v>5</v>
       </c>
       <c r="P86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14000</v>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
         <v>6</v>
       </c>
       <c r="P87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14125</v>
       </c>
     </row>
@@ -2355,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="P88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14250</v>
       </c>
     </row>
@@ -2367,7 +2367,7 @@
         <v>8</v>
       </c>
       <c r="P89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14375</v>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
         <v>9</v>
       </c>
       <c r="P90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14500</v>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
         <v>10</v>
       </c>
       <c r="P91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14625</v>
       </c>
     </row>

</xml_diff>